<commit_message>
corrected factor for decommission of ATM_CCS (-1)
</commit_message>
<xml_diff>
--- a/dev/energyscope_data/core/unit_conversion.xlsx
+++ b/dev/energyscope_data/core/unit_conversion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\mescal\dev\energyscope_data\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F0D3E4-A762-469F-B83D-8FBEF7B9BD18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0136CC72-C619-4FF1-BD8B-7651A434F4B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1286,12 +1286,12 @@
   <dimension ref="A1:F278"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -1385,8 +1385,8 @@
         <v>190</v>
       </c>
       <c r="C5">
-        <f>8760*0.85/1000 / 1000000</f>
-        <v>7.4459999999999995E-6</v>
+        <f>-1*8760*0.85/1000 / 1000000</f>
+        <v>-7.4459999999999995E-6</v>
       </c>
       <c r="D5" t="s">
         <v>195</v>

</xml_diff>